<commit_message>
PLUS DE BUG !!!!!!!!!!!!!!!! CORRECTION TOUT ÇA
</commit_message>
<xml_diff>
--- a/SAE_3_01/fichiers genere/Professeurs_Horaires.xlsx
+++ b/SAE_3_01/fichiers genere/Professeurs_Horaires.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,81 +545,6 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Test2</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>48</v>
-      </c>
-      <c r="E5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>sss</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>16</v>
-      </c>
-      <c r="E6" t="n">
-        <v>16</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>zzz</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>36</v>
-      </c>
-      <c r="D7" t="n">
-        <v>16</v>
-      </c>
-      <c r="E7" t="n">
-        <v>32</v>
-      </c>
-      <c r="F7" t="n">
-        <v>4</v>
-      </c>
-      <c r="G7" t="n">
-        <v>93</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>